<commit_message>
input.py logic changed to waypoints, main.py logic changed to calculate full segments with regard to midnights
</commit_message>
<xml_diff>
--- a/output/spam.xlsx
+++ b/output/spam.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Spam Bacon Eggs Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Spam Bacon Eggs Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Spam Bacon Eggs Sheet'!$A$1:$F$85</definedName>

</xml_diff>

<commit_message>
Updated export json logic
</commit_message>
<xml_diff>
--- a/output/spam.xlsx
+++ b/output/spam.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Vyúčtování služební cesty" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Travelrep CZ" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Vyúčtování služební cesty'!$A$1:$F$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Travelrep CZ'!$A$1:$F$65</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -695,11 +695,7 @@
     </row>
     <row r="25" ht="12" customHeight="1">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>Náklady</t>
-        </is>
-      </c>
+      <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="n"/>
       <c r="D25" s="1" t="n"/>
       <c r="E25" s="1" t="n"/>
@@ -739,7 +735,11 @@
     </row>
     <row r="30" ht="12" customHeight="1">
       <c r="A30" s="1" t="n"/>
-      <c r="B30" s="1" t="n"/>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>Náklady</t>
+        </is>
+      </c>
       <c r="C30" s="1" t="n"/>
       <c r="D30" s="1" t="n"/>
       <c r="E30" s="1" t="n"/>
@@ -776,12 +776,12 @@
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>Plné za.</t>
+          <t>Plné zah.</t>
         </is>
       </c>
       <c r="F32" s="1" t="inlineStr">
         <is>
-          <t>Celk. / den</t>
+          <t>Celk. den</t>
         </is>
       </c>
     </row>
@@ -882,7 +882,7 @@
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="inlineStr">
         <is>
-          <t>Kapesne:</t>
+          <t>Kapesné:</t>
         </is>
       </c>
       <c r="D44" s="1" t="inlineStr">
@@ -965,84 +965,177 @@
       <c r="E50" s="1" t="n"/>
       <c r="F50" s="1" t="n"/>
     </row>
-    <row r="53">
-      <c r="E53" t="inlineStr">
+    <row r="51" ht="12" customHeight="1">
+      <c r="A51" s="1" t="n"/>
+      <c r="B51" s="1" t="n"/>
+      <c r="C51" s="1" t="n"/>
+      <c r="D51" s="1" t="n"/>
+      <c r="E51" s="1" t="n"/>
+      <c r="F51" s="1" t="n"/>
+    </row>
+    <row r="52" ht="12" customHeight="1">
+      <c r="A52" s="1" t="n"/>
+      <c r="B52" s="1" t="n"/>
+      <c r="C52" s="1" t="n"/>
+      <c r="D52" s="1" t="n"/>
+      <c r="E52" s="1" t="n"/>
+      <c r="F52" s="1" t="n"/>
+    </row>
+    <row r="53" ht="12" customHeight="1">
+      <c r="A53" s="1" t="n"/>
+      <c r="B53" s="1" t="n"/>
+      <c r="C53" s="1" t="n"/>
+      <c r="D53" s="1" t="n"/>
+      <c r="E53" s="1" t="inlineStr">
         <is>
           <t>Celkem:</t>
         </is>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="F53" s="1" t="n"/>
+    </row>
+    <row r="54" ht="12" customHeight="1">
+      <c r="A54" s="1" t="inlineStr">
         <is>
           <t>Ostatní</t>
         </is>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="B54" s="1" t="n"/>
+      <c r="C54" s="1" t="n"/>
+      <c r="D54" s="1" t="n"/>
+      <c r="E54" s="1" t="n"/>
+      <c r="F54" s="1" t="n"/>
+    </row>
+    <row r="55" ht="12" customHeight="1">
+      <c r="A55" s="1" t="inlineStr">
         <is>
           <t>Datum</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B55" s="1" t="inlineStr">
         <is>
           <t>Popis</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="C55" s="1" t="n"/>
+      <c r="D55" s="1" t="n"/>
+      <c r="E55" s="1" t="inlineStr">
         <is>
           <t>Doklad č.</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F55" s="1" t="inlineStr">
         <is>
           <t>Částka</t>
         </is>
       </c>
     </row>
-    <row r="61">
-      <c r="E61" t="inlineStr">
+    <row r="56" ht="12" customHeight="1">
+      <c r="A56" s="1" t="n"/>
+      <c r="B56" s="1" t="n"/>
+      <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
+      <c r="E56" s="1" t="n"/>
+      <c r="F56" s="1" t="n"/>
+    </row>
+    <row r="57" ht="12" customHeight="1">
+      <c r="A57" s="1" t="n"/>
+      <c r="B57" s="1" t="n"/>
+      <c r="C57" s="1" t="n"/>
+      <c r="D57" s="1" t="n"/>
+      <c r="E57" s="1" t="n"/>
+      <c r="F57" s="1" t="n"/>
+    </row>
+    <row r="58" ht="12" customHeight="1">
+      <c r="A58" s="1" t="n"/>
+      <c r="B58" s="1" t="n"/>
+      <c r="C58" s="1" t="n"/>
+      <c r="D58" s="1" t="n"/>
+      <c r="E58" s="1" t="n"/>
+      <c r="F58" s="1" t="n"/>
+    </row>
+    <row r="59" ht="12" customHeight="1">
+      <c r="A59" s="1" t="n"/>
+      <c r="B59" s="1" t="n"/>
+      <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
+      <c r="E59" s="1" t="n"/>
+      <c r="F59" s="1" t="n"/>
+    </row>
+    <row r="60" ht="12" customHeight="1">
+      <c r="A60" s="1" t="n"/>
+      <c r="B60" s="1" t="n"/>
+      <c r="C60" s="1" t="n"/>
+      <c r="D60" s="1" t="n"/>
+      <c r="E60" s="1" t="n"/>
+      <c r="F60" s="1" t="n"/>
+    </row>
+    <row r="61" ht="12" customHeight="1">
+      <c r="A61" s="1" t="n"/>
+      <c r="B61" s="1" t="n"/>
+      <c r="C61" s="1" t="n"/>
+      <c r="D61" s="1" t="n"/>
+      <c r="E61" s="1" t="inlineStr">
         <is>
           <t>Celkem:</t>
         </is>
       </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="F61" s="1" t="n"/>
+    </row>
+    <row r="62" ht="12" customHeight="1">
+      <c r="A62" s="1" t="n"/>
+      <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="n"/>
+      <c r="D62" s="1" t="n"/>
+      <c r="E62" s="1" t="n"/>
+      <c r="F62" s="1" t="n"/>
+    </row>
+    <row r="63" ht="12" customHeight="1">
+      <c r="A63" s="1" t="inlineStr">
         <is>
           <t>Zúčtováno dne:</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="B63" s="1" t="n"/>
+      <c r="C63" s="1" t="n"/>
+      <c r="D63" s="1" t="n"/>
+      <c r="E63" s="1" t="inlineStr">
         <is>
           <t>Záloha:</t>
         </is>
       </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="F63" s="1" t="n"/>
+    </row>
+    <row r="64" ht="12" customHeight="1">
+      <c r="A64" s="1" t="inlineStr">
         <is>
           <t>Podpis:</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="inlineStr">
         <is>
           <t>Mezisoučet:</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="D64" s="1" t="n"/>
+      <c r="E64" s="1" t="inlineStr">
         <is>
           <t>Náklady:</t>
         </is>
       </c>
-    </row>
-    <row r="65">
-      <c r="E65" t="inlineStr">
+      <c r="F64" s="1" t="n"/>
+    </row>
+    <row r="65" ht="12" customHeight="1">
+      <c r="A65" s="1" t="n"/>
+      <c r="B65" s="1" t="n"/>
+      <c r="C65" s="1" t="n"/>
+      <c r="D65" s="1" t="n"/>
+      <c r="E65" s="1" t="inlineStr">
         <is>
           <t>K vyplacení:</t>
         </is>
       </c>
+      <c r="F65" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>